<commit_message>
Actualicé archivos de ProjectLibre y Excel para alinear fechas con la entrega.
También agregué nuevos archivos correspondientes a la fase 2.
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\OneDrive\Desktop\Administracion y evaluacion de proyectos de tecnologias de informacion\sistemaInventario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB80759-24A1-49B1-8D55-781CDE2F9D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E7B19C-2D44-4399-96E6-71639622F54E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{9F02E237-A372-4DBD-B752-0CBDF1DD856F}"/>
   </bookViews>
@@ -468,22 +468,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -511,6 +495,22 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -527,20 +527,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF5C85A2-85B6-4366-B0B3-EB506B20E659}" name="Table1" displayName="Table1" ref="A1:I34" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF5C85A2-85B6-4366-B0B3-EB506B20E659}" name="Table1" displayName="Table1" ref="A1:I34" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:I34" xr:uid="{FF5C85A2-85B6-4366-B0B3-EB506B20E659}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{2B3A4301-1449-4043-8CE1-B0376D0898F7}" name="ID" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{94B835CA-25C4-47A3-B7FF-D7FB358E29A7}" name="Actividad" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{DAFD8811-1133-4853-808E-7F121F503A49}" name="Descripción" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{C20657BD-CF98-4B97-BFB1-D931D6F123C9}" name="Responsable" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{0AA79C26-F5AE-4394-8F0E-A4AC401F882C}" name="a" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{B05A6434-6407-4383-A6B0-9850541827EF}" name="m" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{C0581AF5-6F92-4FEF-AADE-FBD0A930DDAC}" name="b" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{756A5C74-F7F1-422A-A6FF-EA7373F4FB21}" name="TE (PERT)" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{2B3A4301-1449-4043-8CE1-B0376D0898F7}" name="ID" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{94B835CA-25C4-47A3-B7FF-D7FB358E29A7}" name="Actividad" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{DAFD8811-1133-4853-808E-7F121F503A49}" name="Descripción" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{C20657BD-CF98-4B97-BFB1-D931D6F123C9}" name="Responsable" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{0AA79C26-F5AE-4394-8F0E-A4AC401F882C}" name="a" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{B05A6434-6407-4383-A6B0-9850541827EF}" name="m" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{C0581AF5-6F92-4FEF-AADE-FBD0A930DDAC}" name="b" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{756A5C74-F7F1-422A-A6FF-EA7373F4FB21}" name="TE (PERT)" dataDxfId="1">
       <calculatedColumnFormula>(Table1[[#This Row],[a]]+(4*Table1[[#This Row],[m]])+Table1[[#This Row],[b]])/6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{11FEA162-4E64-4071-BA4E-BEAF59378811}" name="Dependencias" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{11FEA162-4E64-4071-BA4E-BEAF59378811}" name="Dependencias" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -865,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{571CA8E3-46AA-440C-B867-D5AFC61AA386}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="B27" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1615,17 +1615,17 @@
         <v>68</v>
       </c>
       <c r="E25" s="1">
+        <v>3</v>
+      </c>
+      <c r="F25" s="1">
         <v>4</v>
       </c>
-      <c r="F25" s="1">
+      <c r="G25" s="1">
         <v>5</v>
       </c>
-      <c r="G25" s="1">
-        <v>6</v>
-      </c>
       <c r="H25" s="3">
         <f>(Table1[[#This Row],[a]]+(4*Table1[[#This Row],[m]])+Table1[[#This Row],[b]])/6</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>78</v>
@@ -1738,14 +1738,14 @@
         <v>2</v>
       </c>
       <c r="F29" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G29" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H29" s="3">
         <f>(Table1[[#This Row],[a]]+(4*Table1[[#This Row],[m]])+Table1[[#This Row],[b]])/6</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>90</v>

</xml_diff>

<commit_message>
Correccion de errores del frontend
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\OneDrive\Desktop\Administracion y evaluacion de proyectos de tecnologias de informacion\sistemaInventario\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/312b1f7e5ae81334/Desktop/Administracion y evaluacion de proyectos de tecnologias de informacion/sistemaInventario/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E7B19C-2D44-4399-96E6-71639622F54E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
@@ -865,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{571CA8E3-46AA-440C-B867-D5AFC61AA386}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B27" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>